<commit_message>
Actualización del estado de avance del cronograma, culminación del hito 2
</commit_message>
<xml_diff>
--- a/Desarrollo/SCSE/SCSE-CP.xlsx
+++ b/Desarrollo/SCSE/SCSE-CP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\Gestion\semas\Desarrollo\SCSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe85f0c5da953b39/Desktop/2023-1/Configuracion de software/proyecto/semas/Desarrollo/SCSE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8465184-8C3B-422A-B305-3D1297081EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{A8465184-8C3B-422A-B305-3D1297081EC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CCF7627-B78F-4A40-BC64-AB30DFCDA7BE}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma #1" sheetId="1" r:id="rId1"/>
@@ -1273,17 +1273,17 @@
     <xf numFmtId="9" fontId="23" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1508,24 +1508,24 @@
   </sheetPr>
   <dimension ref="A1:Z1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="E31" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="75.85546875" customWidth="1"/>
-    <col min="3" max="3" width="74.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="81.5703125" customWidth="1"/>
-    <col min="6" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="75.81640625" customWidth="1"/>
+    <col min="3" max="3" width="74.54296875" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" customWidth="1"/>
+    <col min="5" max="5" width="81.54296875" customWidth="1"/>
+    <col min="6" max="7" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="32.25" customHeight="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="63"/>
@@ -1556,10 +1556,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="10"/>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="65"/>
+      <c r="C2" s="66"/>
       <c r="D2" s="11"/>
       <c r="E2" s="10"/>
       <c r="F2" s="12"/>
@@ -1923,7 +1923,7 @@
       <c r="H12" s="32">
         <v>1</v>
       </c>
-      <c r="I12" s="66" t="s">
+      <c r="I12" s="62" t="s">
         <v>25</v>
       </c>
       <c r="J12" s="53"/>
@@ -2135,7 +2135,7 @@
       <c r="H17" s="32">
         <v>1</v>
       </c>
-      <c r="I17" s="66" t="s">
+      <c r="I17" s="62" t="s">
         <v>43</v>
       </c>
       <c r="J17" s="53"/>
@@ -2307,7 +2307,7 @@
       <c r="H21" s="32">
         <v>1</v>
       </c>
-      <c r="I21" s="66" t="s">
+      <c r="I21" s="62" t="s">
         <v>59</v>
       </c>
       <c r="J21" s="53"/>
@@ -2435,7 +2435,7 @@
       <c r="H24" s="32">
         <v>1</v>
       </c>
-      <c r="I24" s="66" t="s">
+      <c r="I24" s="62" t="s">
         <v>72</v>
       </c>
       <c r="J24" s="53"/>
@@ -2647,7 +2647,7 @@
       <c r="H29" s="32">
         <v>1</v>
       </c>
-      <c r="I29" s="66" t="s">
+      <c r="I29" s="62" t="s">
         <v>88</v>
       </c>
       <c r="J29" s="53"/>
@@ -2771,7 +2771,7 @@
       <c r="H32" s="32">
         <v>1</v>
       </c>
-      <c r="I32" s="66" t="s">
+      <c r="I32" s="62" t="s">
         <v>94</v>
       </c>
       <c r="J32" s="53"/>
@@ -3359,7 +3359,7 @@
         <v>45047</v>
       </c>
       <c r="H46" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46" s="63"/>
       <c r="J46" s="53"/>
@@ -3397,9 +3397,9 @@
         <v>45079</v>
       </c>
       <c r="H47" s="48">
-        <v>0</v>
-      </c>
-      <c r="I47" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="I47" s="62" t="s">
         <v>116</v>
       </c>
       <c r="J47" s="53"/>
@@ -3821,7 +3821,7 @@
       <c r="H57" s="32">
         <v>0</v>
       </c>
-      <c r="I57" s="66" t="s">
+      <c r="I57" s="62" t="s">
         <v>127</v>
       </c>
       <c r="J57" s="53"/>
@@ -30782,16 +30782,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="I21:I23"/>
     <mergeCell ref="I24:I28"/>
     <mergeCell ref="I29:I31"/>
     <mergeCell ref="I32:I46"/>
     <mergeCell ref="I47:I48"/>
     <mergeCell ref="I57:I59"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="I21:I23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -30810,12 +30810,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" customWidth="1"/>
-    <col min="4" max="6" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="3" max="3" width="38.1796875" customWidth="1"/>
+    <col min="4" max="6" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="15.75" customHeight="1"/>
@@ -31917,9 +31917,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="12.5703125" customWidth="1"/>
+    <col min="1" max="6" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Correccion de nombre de integrante y herramientas que se utilizan
</commit_message>
<xml_diff>
--- a/Desarrollo/SCSE/SCSE-CP.xlsx
+++ b/Desarrollo/SCSE/SCSE-CP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe85f0c5da953b39/Desktop/2023-1/Configuracion de software/proyecto/semas/Desarrollo/SCSE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{A8465184-8C3B-422A-B305-3D1297081EC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CCF7627-B78F-4A40-BC64-AB30DFCDA7BE}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{A8465184-8C3B-422A-B305-3D1297081EC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{84B32EE3-9FB3-48DE-89C2-EF107A3B2ED9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="910" windowWidth="15350" windowHeight="9000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma #1" sheetId="1" r:id="rId1"/>
@@ -515,9 +515,6 @@
     <t>Hito 3 - Fin del Sprint #3</t>
   </si>
   <si>
-    <t>Herramienta: Mercurial</t>
-  </si>
-  <si>
     <t>GRUPO 3</t>
   </si>
   <si>
@@ -545,9 +542,6 @@
     <t>Administrador de base de datos</t>
   </si>
   <si>
-    <t>Felix Huayhua Alex Patrick Julian</t>
-  </si>
-  <si>
     <t>Huaman Ortiz Emerson Raul</t>
   </si>
   <si>
@@ -573,6 +567,12 @@
   </si>
   <si>
     <t>Asegurador de Calidad</t>
+  </si>
+  <si>
+    <t>Herramienta:Git y Github</t>
+  </si>
+  <si>
+    <t>Felix Huayhua Axel Patrick Julian</t>
   </si>
 </sst>
 </file>
@@ -1273,17 +1273,17 @@
     <xf numFmtId="9" fontId="23" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1508,7 +1508,7 @@
   </sheetPr>
   <dimension ref="A1:Z1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E31" workbookViewId="0">
+    <sheetView topLeftCell="E28" workbookViewId="0">
       <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
@@ -1525,7 +1525,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="32.25" customHeight="1">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="63"/>
@@ -1556,10 +1556,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="10"/>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="66"/>
+      <c r="C2" s="65"/>
       <c r="D2" s="11"/>
       <c r="E2" s="10"/>
       <c r="F2" s="12"/>
@@ -1923,7 +1923,7 @@
       <c r="H12" s="32">
         <v>1</v>
       </c>
-      <c r="I12" s="62" t="s">
+      <c r="I12" s="66" t="s">
         <v>25</v>
       </c>
       <c r="J12" s="53"/>
@@ -2135,7 +2135,7 @@
       <c r="H17" s="32">
         <v>1</v>
       </c>
-      <c r="I17" s="62" t="s">
+      <c r="I17" s="66" t="s">
         <v>43</v>
       </c>
       <c r="J17" s="53"/>
@@ -2307,7 +2307,7 @@
       <c r="H21" s="32">
         <v>1</v>
       </c>
-      <c r="I21" s="62" t="s">
+      <c r="I21" s="66" t="s">
         <v>59</v>
       </c>
       <c r="J21" s="53"/>
@@ -2435,7 +2435,7 @@
       <c r="H24" s="32">
         <v>1</v>
       </c>
-      <c r="I24" s="62" t="s">
+      <c r="I24" s="66" t="s">
         <v>72</v>
       </c>
       <c r="J24" s="53"/>
@@ -2647,7 +2647,7 @@
       <c r="H29" s="32">
         <v>1</v>
       </c>
-      <c r="I29" s="62" t="s">
+      <c r="I29" s="66" t="s">
         <v>88</v>
       </c>
       <c r="J29" s="53"/>
@@ -2771,7 +2771,7 @@
       <c r="H32" s="32">
         <v>1</v>
       </c>
-      <c r="I32" s="62" t="s">
+      <c r="I32" s="66" t="s">
         <v>94</v>
       </c>
       <c r="J32" s="53"/>
@@ -3399,7 +3399,7 @@
       <c r="H47" s="48">
         <v>1</v>
       </c>
-      <c r="I47" s="62" t="s">
+      <c r="I47" s="66" t="s">
         <v>116</v>
       </c>
       <c r="J47" s="53"/>
@@ -3821,7 +3821,7 @@
       <c r="H57" s="32">
         <v>0</v>
       </c>
-      <c r="I57" s="62" t="s">
+      <c r="I57" s="66" t="s">
         <v>127</v>
       </c>
       <c r="J57" s="53"/>
@@ -30782,16 +30782,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I24:I28"/>
+    <mergeCell ref="I29:I31"/>
+    <mergeCell ref="I32:I46"/>
+    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="I57:I59"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="I12:I16"/>
     <mergeCell ref="I17:I19"/>
     <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I28"/>
-    <mergeCell ref="I29:I31"/>
-    <mergeCell ref="I32:I46"/>
-    <mergeCell ref="I47:I48"/>
-    <mergeCell ref="I57:I59"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -30808,7 +30808,9 @@
   </sheetPr>
   <dimension ref="B1:C1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -30821,94 +30823,94 @@
     <row r="1" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="2" spans="2:3" ht="15.75" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="2:3" ht="15.75" customHeight="1">
       <c r="B3" s="67" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="68"/>
     </row>
     <row r="4" spans="2:3" ht="15.75" customHeight="1">
       <c r="B4" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>153</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" customHeight="1">
       <c r="B6" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>155</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" customHeight="1">
       <c r="B7" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" customHeight="1">
       <c r="B8" s="7" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" customHeight="1">
       <c r="B10" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15.75" customHeight="1">
       <c r="B13" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15.75" customHeight="1"/>
@@ -31915,7 +31917,7 @@
   </sheetPr>
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>